<commit_message>
updated non *-tasks, update sigma
</commit_message>
<xml_diff>
--- a/Doku/Abschätzung.xlsx
+++ b/Doku/Abschätzung.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nick\Documents\GitHub\ASCET_Projekt\Doku\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E1A0A84-6795-4DAA-BA7F-460BF6F66E17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92D2E8FE-4CAB-4B84-894E-2D00B12E0EC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="332" xr2:uid="{3BD75EA3-47ED-4B45-9003-11B3070BA44C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Aufgaben [min]</t>
   </si>
@@ -100,6 +100,12 @@
   </si>
   <si>
     <t>TrafficLight Modul implementieren</t>
+  </si>
+  <si>
+    <t>Total time</t>
+  </si>
+  <si>
+    <t>2-Sigma Range</t>
   </si>
 </sst>
 </file>
@@ -109,7 +115,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -123,16 +129,38 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -140,18 +168,39 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1"/>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Ausgabe" xfId="1" builtinId="21"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -466,315 +515,321 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{430D41D9-55EE-4ED9-B8A0-34F7167870DA}">
   <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="41.42578125" customWidth="1"/>
-    <col min="6" max="6" width="6.5703125" customWidth="1"/>
-    <col min="7" max="7" width="6.85546875" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" customWidth="1"/>
+    <col min="4" max="4" width="12" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" customWidth="1"/>
+    <col min="6" max="6" width="8.140625" customWidth="1"/>
+    <col min="7" max="7" width="8" customWidth="1"/>
     <col min="10" max="10" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="4">
         <v>38</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="4">
         <v>5</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="4">
         <v>10</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="4">
         <v>25</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="5">
         <f>(C2+4*D2+E2)/6</f>
         <v>11.666666666666666</v>
       </c>
-      <c r="G2" s="4">
+      <c r="G2" s="5">
         <f>(E2-C2)^2/36</f>
         <v>11.111111111111111</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="4">
         <v>8</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="4">
         <v>5</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="4">
         <v>10</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="4">
         <v>20</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="5">
         <f t="shared" ref="F3:F16" si="0">(C3+4*D3+E3)/6</f>
         <v>10.833333333333334</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="5">
         <f t="shared" ref="G3:G16" si="1">(E3-C3)^2/36</f>
         <v>6.25</v>
       </c>
       <c r="J3" s="2"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="4" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="4">
         <v>18</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="4">
         <v>10</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="4">
         <v>12</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="4">
         <v>20</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="5">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="5">
         <f t="shared" si="1"/>
         <v>2.7777777777777777</v>
       </c>
       <c r="J4" s="2"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="5" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="4">
         <v>29</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="4">
         <v>20</v>
       </c>
-      <c r="D5">
-        <v>30</v>
-      </c>
-      <c r="E5">
+      <c r="D5" s="4">
+        <v>30</v>
+      </c>
+      <c r="E5" s="4">
         <v>45</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="5">
         <f t="shared" si="0"/>
         <v>30.833333333333332</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="5">
         <f t="shared" si="1"/>
         <v>17.361111111111111</v>
       </c>
       <c r="J5" s="2"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="6" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="4">
         <v>131</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="4">
         <v>60</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="4">
         <v>100</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="4">
         <v>150</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="5">
         <f t="shared" si="0"/>
         <v>101.66666666666667</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="5">
         <f t="shared" si="1"/>
         <v>225</v>
       </c>
       <c r="J6" s="2"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="7" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="4">
         <v>48</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="4">
         <v>15</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="4">
         <v>35</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="4">
         <v>45</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="5">
         <f t="shared" si="0"/>
         <v>33.333333333333336</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="5">
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
       <c r="J7" s="2"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+    <row r="8" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="4">
         <v>72</v>
       </c>
-      <c r="C8">
-        <v>30</v>
-      </c>
-      <c r="D8">
+      <c r="C8" s="4">
+        <v>30</v>
+      </c>
+      <c r="D8" s="4">
         <v>45</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="4">
         <v>100</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="5">
         <f t="shared" si="0"/>
         <v>51.666666666666664</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8" s="5">
         <f t="shared" si="1"/>
         <v>136.11111111111111</v>
       </c>
       <c r="J8" s="2"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    <row r="9" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="4">
         <v>116</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="4">
         <v>90</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="4">
         <v>150</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="4">
         <v>60</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F9" s="5">
         <f t="shared" si="0"/>
         <v>125</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9" s="5">
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
       <c r="J9" s="2"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+    <row r="10" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B10">
-        <v>30</v>
-      </c>
-      <c r="C10">
+      <c r="B10" s="4">
+        <v>30</v>
+      </c>
+      <c r="C10" s="4">
         <v>10</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="4">
         <v>15</v>
       </c>
-      <c r="E10">
-        <v>30</v>
-      </c>
-      <c r="F10" s="4">
+      <c r="E10" s="4">
+        <v>30</v>
+      </c>
+      <c r="F10" s="5">
         <f t="shared" si="0"/>
         <v>16.666666666666668</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10" s="5">
         <f t="shared" si="1"/>
         <v>11.111111111111111</v>
       </c>
       <c r="J10" s="2"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="11" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C11">
+      <c r="B11" s="4"/>
+      <c r="C11" s="4">
         <v>20</v>
       </c>
-      <c r="D11">
-        <v>30</v>
-      </c>
-      <c r="E11">
+      <c r="D11" s="4">
+        <v>30</v>
+      </c>
+      <c r="E11" s="4">
         <v>40</v>
       </c>
-      <c r="F11" s="4">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="G11" s="4">
+      <c r="F11" s="5">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="G11" s="5">
         <f t="shared" si="1"/>
         <v>11.111111111111111</v>
       </c>
       <c r="J11" s="2"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+    <row r="12" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C12">
+      <c r="B12" s="4"/>
+      <c r="C12" s="4">
         <v>20</v>
       </c>
-      <c r="D12">
-        <v>30</v>
-      </c>
-      <c r="E12">
+      <c r="D12" s="4">
+        <v>30</v>
+      </c>
+      <c r="E12" s="4">
         <v>40</v>
       </c>
-      <c r="F12" s="4">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="G12" s="4">
+      <c r="F12" s="5">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="G12" s="5">
         <f t="shared" si="1"/>
         <v>11.111111111111111</v>
       </c>
@@ -782,24 +837,25 @@
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+    <row r="13" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C13">
+      <c r="B13" s="4"/>
+      <c r="C13" s="4">
         <v>20</v>
       </c>
-      <c r="D13">
-        <v>30</v>
-      </c>
-      <c r="E13">
+      <c r="D13" s="4">
+        <v>30</v>
+      </c>
+      <c r="E13" s="4">
         <v>40</v>
       </c>
-      <c r="F13" s="4">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="G13" s="4">
+      <c r="F13" s="5">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="G13" s="5">
         <f t="shared" si="1"/>
         <v>11.111111111111111</v>
       </c>
@@ -807,84 +863,107 @@
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+    <row r="14" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C14">
+      <c r="B14" s="4">
+        <v>172</v>
+      </c>
+      <c r="C14" s="4">
         <v>100</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="4">
         <v>120</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="4">
         <v>160</v>
       </c>
-      <c r="F14" s="4">
+      <c r="F14" s="5">
         <f t="shared" si="0"/>
         <v>123.33333333333333</v>
       </c>
-      <c r="G14" s="4">
+      <c r="G14" s="5">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+    <row r="15" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C15">
+      <c r="B15" s="4"/>
+      <c r="C15" s="4">
         <v>20</v>
       </c>
-      <c r="D15">
-        <v>30</v>
-      </c>
-      <c r="E15">
+      <c r="D15" s="4">
+        <v>30</v>
+      </c>
+      <c r="E15" s="4">
         <v>40</v>
       </c>
-      <c r="F15" s="4">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="G15" s="4">
+      <c r="F15" s="5">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="G15" s="5">
         <f t="shared" si="1"/>
         <v>11.111111111111111</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+    <row r="16" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C16">
-        <v>30</v>
-      </c>
-      <c r="D16">
+      <c r="B16" s="4"/>
+      <c r="C16" s="4">
+        <v>30</v>
+      </c>
+      <c r="D16" s="4">
         <v>45</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="4">
         <v>50</v>
       </c>
-      <c r="F16" s="4">
+      <c r="F16" s="5">
         <f t="shared" si="0"/>
         <v>43.333333333333336</v>
       </c>
-      <c r="G16" s="4">
+      <c r="G16" s="5">
         <f t="shared" si="1"/>
         <v>11.111111111111111</v>
       </c>
     </row>
-    <row r="17" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F17">
+    <row r="17" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="4">
+        <f>SUM(B2:B16)</f>
+        <v>662</v>
+      </c>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="5">
         <f>SUM(F2:F16)</f>
         <v>681.33333333333337</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="5">
         <f>SUM(G2:G16)</f>
         <v>615.2777777777776</v>
       </c>
     </row>
-    <row r="18" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F18" s="1">
+    <row r="18" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="D18" s="6"/>
+      <c r="E18" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F18" s="5">
+        <f>F17-2*(G17^0.5)</f>
+        <v>631.72374644620936</v>
+      </c>
+      <c r="G18" s="5">
         <f>F17+2*(G17^0.5)</f>
         <v>730.94292022045738</v>
       </c>

</xml_diff>